<commit_message>
PIC16 Dev Kit v2.1 - change logo, add fiducial
</commit_message>
<xml_diff>
--- a/HW/Product/BoM/PIC16DevKit.xlsx
+++ b/HW/Product/BoM/PIC16DevKit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\SAMPIDevKit\PIC16DevKit\PIC16F1887x\HW\Product\BoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A945E227-F589-42D4-8B0F-31F746B08607}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45943BD-987C-461D-9C37-81A2A4E28ECD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{B27DB8C2-8D4B-45E4-AB09-F38A4E487824}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{B27DB8C2-8D4B-45E4-AB09-F38A4E487824}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="152">
   <si>
     <t>References</t>
   </si>
@@ -473,6 +473,18 @@
   </si>
   <si>
     <t>MCP1702T-3302E/CB</t>
+  </si>
+  <si>
+    <t>Number Of Pads</t>
+  </si>
+  <si>
+    <t>Pad/Unit</t>
+  </si>
+  <si>
+    <t>TH/Unit</t>
+  </si>
+  <si>
+    <t>Number Of THs</t>
   </si>
 </sst>
 </file>
@@ -583,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -737,6 +749,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1055,9 +1070,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF4A555-F70F-4E5F-B41F-99C917195BA0}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,6 +2060,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="52">
+        <f>SUM(B2:B39)</f>
+        <v>75</v>
+      </c>
       <c r="F40" s="15" t="s">
         <v>83</v>
       </c>
@@ -2080,26 +2099,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10D57EF-1891-4870-B3A7-D95990B0FA3B}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="62.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="95.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="17.42578125" style="1"/>
+    <col min="8" max="8" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="17.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>65</v>
       </c>
@@ -2121,8 +2144,20 @@
       <c r="G1" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2145,8 +2180,22 @@
         <f>PRODUCT(B2,F2)</f>
         <v>1400</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="1">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1">
+        <f>I2*B2</f>
+        <v>8</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <f>K2*B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2169,8 +2218,22 @@
         <f t="shared" ref="G3:G35" si="0">PRODUCT(B3,F3)</f>
         <v>3920</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J35" si="1">I3*B3</f>
+        <v>8</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L35" si="2">K3*B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2193,8 +2256,22 @@
         <f t="shared" si="0"/>
         <v>1440</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2217,8 +2294,22 @@
         <f t="shared" si="0"/>
         <v>3060</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2241,8 +2332,22 @@
         <f t="shared" si="0"/>
         <v>2940</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2265,8 +2370,22 @@
         <f t="shared" si="0"/>
         <v>260</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2289,8 +2408,22 @@
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2313,8 +2446,22 @@
         <f t="shared" si="0"/>
         <v>260</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2337,8 +2484,22 @@
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -2361,8 +2522,22 @@
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="26">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K11" s="26">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -2385,8 +2560,22 @@
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="26">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K12" s="26">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2409,8 +2598,22 @@
         <f t="shared" si="0"/>
         <v>680</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="1">
+        <v>9</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2433,8 +2636,22 @@
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>35</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>16</v>
       </c>
@@ -2457,8 +2674,22 @@
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>18</v>
       </c>
@@ -2481,8 +2712,22 @@
         <f t="shared" si="0"/>
         <v>10800</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="26">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="26">
+        <v>6</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>20</v>
       </c>
@@ -2505,8 +2750,22 @@
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="26">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K17" s="26">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>21</v>
       </c>
@@ -2529,8 +2788,22 @@
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="26">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K18" s="26">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>22</v>
       </c>
@@ -2553,8 +2826,22 @@
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>23</v>
       </c>
@@ -2577,8 +2864,22 @@
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>24</v>
       </c>
@@ -2601,8 +2902,22 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>25</v>
       </c>
@@ -2625,8 +2940,22 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>26</v>
       </c>
@@ -2649,8 +2978,22 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="26">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K23" s="26">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>27</v>
       </c>
@@ -2673,8 +3016,22 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="26">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K24" s="26">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
         <v>28</v>
       </c>
@@ -2697,8 +3054,22 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <v>29</v>
       </c>
@@ -2722,8 +3093,22 @@
         <f t="shared" si="0"/>
         <v>6500</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="45">
         <v>30</v>
       </c>
@@ -2749,8 +3134,22 @@
       <c r="H27" s="51" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1">
+        <v>3</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <v>31</v>
       </c>
@@ -2773,8 +3172,22 @@
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="1">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>32</v>
       </c>
@@ -2797,8 +3210,22 @@
         <f t="shared" si="0"/>
         <v>14000</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="26">
+        <v>8</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K29" s="26">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>33</v>
       </c>
@@ -2822,8 +3249,22 @@
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="1">
+        <v>8</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
         <v>34</v>
       </c>
@@ -2846,8 +3287,22 @@
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="26">
+        <v>6</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K31" s="26">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <v>35</v>
       </c>
@@ -2871,8 +3326,22 @@
         <f t="shared" si="0"/>
         <v>52000</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="1">
+        <v>32</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33">
         <v>36</v>
       </c>
@@ -2895,8 +3364,22 @@
         <f t="shared" si="0"/>
         <v>22000</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="26">
+        <v>6</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K33" s="26">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
         <v>37</v>
       </c>
@@ -2920,8 +3403,22 @@
         <f t="shared" si="0"/>
         <v>48000</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="1">
+        <v>44</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>67</v>
       </c>
@@ -2944,8 +3441,23 @@
         <f t="shared" si="0"/>
         <v>23000</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="52"/>
       <c r="F36" s="15" t="s">
         <v>83</v>
       </c>
@@ -2953,8 +3465,16 @@
         <f>SUM(G2:G35)</f>
         <v>286804</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="1">
+        <f>SUM(J2:J35)</f>
+        <v>239</v>
+      </c>
+      <c r="L36" s="1">
+        <f>SUM(L2:L35)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F37" s="15" t="s">
         <v>87</v>
       </c>
@@ -2963,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F38" s="4" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
PIC16 Dev Kit v2.1 - layout update 3
</commit_message>
<xml_diff>
--- a/HW/Product/BoM/PIC16DevKit.xlsx
+++ b/HW/Product/BoM/PIC16DevKit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\SAMPIDevKit\PIC16DevKit\PIC16F1887x\HW\Product\BoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C83FCC0-4B0E-4BC7-BF22-3A0AC35CAF12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0520652-99F6-43DD-9F6F-6F1DE12BF144}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{ACE22CD8-8350-43B9-B6FE-84662C69CD7D}"/>
+    <workbookView xWindow="-20610" yWindow="-90" windowWidth="20730" windowHeight="11760" xr2:uid="{ACE22CD8-8350-43B9-B6FE-84662C69CD7D}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>References</t>
   </si>
@@ -45,9 +45,6 @@
     <t>CAP CER 0.1UF 16V X7R 0603</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>CAP TANT 220UF 20% 6.3V 1411</t>
   </si>
   <si>
@@ -228,12 +225,6 @@
     <t>Q1, Q2</t>
   </si>
   <si>
-    <t>C1, C3, C12, C21</t>
-  </si>
-  <si>
-    <t>C4, C5, C6, C7, C9, C10, C11, C13, C14, C15, C16, C17, C19, C20, C25</t>
-  </si>
-  <si>
     <t>R1, R10, R14, R23, R26</t>
   </si>
   <si>
@@ -268,6 +259,21 @@
   </si>
   <si>
     <t>Crossed P/N</t>
+  </si>
+  <si>
+    <t>C1, C3, C12, C21, C26, C27</t>
+  </si>
+  <si>
+    <t>C8, C23</t>
+  </si>
+  <si>
+    <t>C4, C5, C6, C7, C9, C10, C11, C13, C14, C15, C16, C17, C19, C20, C24, C25</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 300MA SOT23-5</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -439,14 +445,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -766,54 +775,56 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K37" sqref="A1:K37"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="5.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" s="19"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="17" t="s">
         <v>2</v>
       </c>
@@ -823,10 +834,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/CC0805ZKY5V6BB226/5884300","CC0805ZKY5V6BB226")</f>
@@ -841,7 +852,7 @@
       </c>
       <c r="H2" s="10">
         <f t="shared" ref="H2:H11" si="0">G2*B2</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I2" s="10">
         <v>0</v>
@@ -859,10 +870,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/CC0603JRX7R7BB104/5195185","CC0603JRX7R7BB104")</f>
@@ -877,13 +888,13 @@
       </c>
       <c r="H3" s="10">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I3" s="10">
         <v>0</v>
       </c>
       <c r="J3" s="10">
-        <f t="shared" ref="J3:J36" si="1">I3*B3</f>
+        <f t="shared" ref="J3:J37" si="1">I3*B3</f>
         <v>0</v>
       </c>
       <c r="K3" s="8">
@@ -895,10 +906,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="D4" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/vishay-sprague/TMCMB0J227MTRF/10107352","TMCMB0J227MTRF")</f>
@@ -906,14 +917,14 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="10">
         <v>2</v>
       </c>
       <c r="H4" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4" s="10">
         <v>0</v>
@@ -934,7 +945,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/CC0603JRX7R7BB105/7164369","CC0603JRX7R7BB105")</f>
@@ -970,7 +981,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/AC0603JR-071KL/5896388","AC0603JR-071KL")</f>
@@ -978,7 +989,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="10">
         <v>2</v>
@@ -1006,7 +1017,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D7" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/AC0603JR-0710KL/2827830","AC0603JR-0710KL")</f>
@@ -1014,7 +1025,7 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="10">
         <v>2</v>
@@ -1042,7 +1053,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/AC0603JR-074K7L/5896467","AC0603JR-074K7L")</f>
@@ -1050,7 +1061,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="10">
         <v>2</v>
@@ -1078,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/RC0603FR-0775KL/727378","RC0603FR-0775KL")</f>
@@ -1086,7 +1097,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="11">
         <v>2</v>
@@ -1114,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/RC0603FR-0740K2L/727221","RC0603FR-0740K2L")</f>
@@ -1122,7 +1133,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="11">
         <v>2</v>
@@ -1150,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/RC0603FR-077K68L/727367","RC0603FR-077K68L")</f>
@@ -1158,7 +1169,7 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="11">
         <v>2</v>
@@ -1186,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/yageo/AC0603JR-072K2L/5896418","AC0603JR-072K2L")</f>
@@ -1194,7 +1205,7 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="11">
         <v>2</v>
@@ -1222,7 +1233,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/diodes-incorporated/AP2210N-3-3TRG1/4470822","AP2210N-3.3TRG1")</f>
@@ -1230,13 +1241,13 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" s="11">
         <v>3</v>
       </c>
       <c r="H13" s="10">
-        <f t="shared" ref="H13:H36" si="2">G13*B13</f>
+        <f t="shared" ref="H13:H37" si="2">G13*B13</f>
         <v>3</v>
       </c>
       <c r="I13" s="11">
@@ -1258,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/microchip-technology/MCP9701T-E-TT/1987445","MCP9700T-H/LT")</f>
@@ -1266,7 +1277,7 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="11">
         <v>3</v>
@@ -1294,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/microchip-technology/SST25VF040B-50-4C-SAF/4740879","SST25VF040B-50-4C-SAF")</f>
@@ -1302,7 +1313,7 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="11">
         <v>8</v>
@@ -1330,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/micro-crystal-ag/RV-3028-C7-32-768KHZ-1PPM-TA-QC/10431070","RV-3028-C7 32.768KHZ 1PPM-TA-QC")</f>
@@ -1338,7 +1349,7 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="11">
         <v>8</v>
@@ -1366,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/monolithic-power-systems-inc/MP1470GJ-Z/9555284","MP1470GJ-Z")</f>
@@ -1374,7 +1385,7 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="11">
         <v>6</v>
@@ -1402,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/microchip-technology/PIC32MM0064GPM028-I-M6/8037777","PIC32MM0064GPM028-I/M6")</f>
@@ -1410,7 +1421,7 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="11">
         <v>32</v>
@@ -1438,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/nexperia-usa-inc/74AVC2T45DC-125/1692558","74AVC2T45DC,125")</f>
@@ -1446,7 +1457,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="11">
         <v>8</v>
@@ -1474,7 +1485,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="3" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/microchip-technology/PIC16F18876-I-PT/6192935","PIC16F18876-I/PT")</f>
@@ -1482,7 +1493,7 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="11">
         <v>44</v>
@@ -1507,25 +1518,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/toshiba-semiconductor-and-storage/SSM3J378R-LF/9866021","SSM3J378R,LF")</f>
-        <v>SSM3J378R,LF</v>
+        <v>81</v>
+      </c>
+      <c r="D21" s="21" t="str">
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/microchip-technology/MIC5504-3-3YM5-TR/4864018","MIC5504-3.3YM5-TR")</f>
+        <v>MIC5504-3.3YM5-TR</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="G21" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H21" s="10">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I21" s="11">
         <v>0</v>
@@ -1535,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="8">
-        <v>0.30199999999999999</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1543,25 +1554,25 @@
         <v>21</v>
       </c>
       <c r="B22" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060BS75000/4489895","150060BS75000")</f>
-        <v>150060BS75000</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/toshiba-semiconductor-and-storage/SSM3J378R-LF/9866021","SSM3J378R,LF")</f>
+        <v>SSM3J378R,LF</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G22" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I22" s="11">
         <v>0</v>
@@ -1571,7 +1582,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="8">
-        <v>0.16</v>
+        <v>0.30199999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1579,25 +1590,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060SS75000/4489903","150060SS75000")</f>
-        <v>150060SS75000</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060BS75000/4489895","150060BS75000")</f>
+        <v>150060BS75000</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G23" s="11">
         <v>2</v>
       </c>
       <c r="H23" s="10">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I23" s="11">
         <v>0</v>
@@ -1607,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1615,25 +1626,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060VS75000/4489906","150060VS75000")</f>
-        <v>150060VS75000</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060SS75000/4489903","150060SS75000")</f>
+        <v>150060SS75000</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G24" s="11">
         <v>2</v>
       </c>
       <c r="H24" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I24" s="11">
         <v>0</v>
@@ -1654,15 +1665,15 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060YS75000/4489909","150060YS75000")</f>
-        <v>150060YS75000</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060VS75000/4489906","150060VS75000")</f>
+        <v>150060VS75000</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G25" s="11">
         <v>2</v>
@@ -1690,15 +1701,15 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/smc-diode-solutions/1N4148WSTR/6022449","1N4148WSTR")</f>
-        <v>1N4148WSTR</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/würth-elektronik/150060YS75000/4489909","150060YS75000")</f>
+        <v>150060YS75000</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G26" s="11">
         <v>2</v>
@@ -1715,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="8">
-        <v>0.121</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1726,15 +1737,15 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f>HYPERLINK("https://www.mouser.vn/ProductDetail/Panjit/SK26_R1_00001?qs=sPbYRqrBIVnCfhq3ypDoOA%3D%3D","SK26_R1_00001")</f>
-        <v>SK26_R1_00001</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/smc-diode-solutions/1N4148WSTR/6022449","1N4148WSTR")</f>
+        <v>1N4148WSTR</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="G27" s="11">
         <v>2</v>
@@ -1751,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="8">
-        <v>0.36</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1759,25 +1770,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/c-k/PTS810-SJG-250-SMTR-LFS/4176612","PTS810 SJG 250 SMTR LFS")</f>
-        <v>PTS810 SJG 250 SMTR LFS</v>
+        <f>HYPERLINK("https://www.mouser.vn/ProductDetail/Panjit/SK26_R1_00001?qs=sPbYRqrBIVnCfhq3ypDoOA%3D%3D","SK26_R1_00001")</f>
+        <v>SK26_R1_00001</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G28" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H28" s="10">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I28" s="11">
         <v>0</v>
@@ -1787,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="8">
-        <v>0.35399999999999998</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1795,25 +1806,25 @@
         <v>28</v>
       </c>
       <c r="B29" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/bel-fuse-inc/0ZCG0050AF2C/4156100","0ZCG0050AF2C")</f>
-        <v>0ZCG0050AF2C</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/c-k/PTS810-SJG-250-SMTR-LFS/4176612","PTS810 SJG 250 SMTR LFS")</f>
+        <v>PTS810 SJG 250 SMTR LFS</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G29" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H29" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I29" s="11">
         <v>0</v>
@@ -1823,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="8">
-        <v>0.107</v>
+        <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1834,22 +1845,22 @@
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/amphenol-icc-fci/10118192-0002LF/6817756","10118192-0002LF")</f>
-        <v>10118192-0002LF</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/bel-fuse-inc/0ZCG0050AF2C/4156100","0ZCG0050AF2C")</f>
+        <v>0ZCG0050AF2C</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G30" s="11">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H30" s="10">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I30" s="11">
         <v>0</v>
@@ -1859,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="8">
-        <v>0.44</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1867,35 +1878,35 @@
         <v>30</v>
       </c>
       <c r="B31" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/RS1-10-G/9832059","RS1-10-G")</f>
-        <v>RS1-10-G</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/amphenol-icc-fci/10118192-0002LF/6817756","10118192-0002LF")</f>
+        <v>10118192-0002LF</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G31" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H31" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I31" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J31" s="10">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K31" s="8">
-        <v>0.58299999999999996</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1903,18 +1914,18 @@
         <v>31</v>
       </c>
       <c r="B32" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/RS1-07-G/9832045","RS1-07-G")</f>
-        <v>RS1-07-G</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/RS1-10-G/9832059","RS1-10-G")</f>
+        <v>RS1-10-G</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G32" s="11">
         <v>0</v>
@@ -1924,14 +1935,14 @@
         <v>0</v>
       </c>
       <c r="I32" s="11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J32" s="10">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="K32" s="8">
-        <v>0.44500000000000001</v>
+        <v>0.58299999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1942,15 +1953,15 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/RS1-08-G/9832056","RS1-08-G")</f>
-        <v>RS1-08-G</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/RS1-07-G/9832045","RS1-07-G")</f>
+        <v>RS1-07-G</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G33" s="11">
         <v>0</v>
@@ -1960,14 +1971,14 @@
         <v>0</v>
       </c>
       <c r="I33" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J33" s="10">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K33" s="8">
-        <v>0.46700000000000003</v>
+        <v>0.44500000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1978,15 +1989,15 @@
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/HRS-2B-10-GA/9832984","HRS-2B-10-GA")</f>
-        <v>HRS-2B-10-GA</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/RS1-08-G/9832056","RS1-08-G")</f>
+        <v>RS1-08-G</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G34" s="11">
         <v>0</v>
@@ -2003,7 +2014,7 @@
         <v>8</v>
       </c>
       <c r="K34" s="8">
-        <v>0.38900000000000001</v>
+        <v>0.46700000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2014,32 +2025,32 @@
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>HYPERLINK("https://www.digikey.com/en/products/detail/bourns-inc/SDE0604A-6R8M/5030882","SDE0604A-6R8M")</f>
-        <v>SDE0604A-6R8M</v>
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/adam-tech/HRS-2B-10-GA/9832984","HRS-2B-10-GA")</f>
+        <v>HRS-2B-10-GA</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G35" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H35" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I35" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J35" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K35" s="8">
-        <v>0.59299999999999997</v>
+        <v>0.38900000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2050,21 +2061,22 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/bourns-inc/SDE0604A-6R8M/5030882","SDE0604A-6R8M")</f>
+        <v>SDE0604A-6R8M</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G36" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I36" s="11">
         <v>0</v>
@@ -2074,34 +2086,69 @@
         <v>0</v>
       </c>
       <c r="K36" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="13">
-        <f>SUM(B2:B36)</f>
-        <v>68</v>
-      </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15">
-        <f>SUM(H2:H36)</f>
-        <v>233</v>
-      </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15">
-        <f>SUM(J2:J36)</f>
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="11">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="11">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="13">
+        <f>SUM(B2:B37)</f>
+        <v>73</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15">
+        <f>SUM(H2:H37)</f>
+        <v>246</v>
+      </c>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15">
+        <f>SUM(J2:J37)</f>
         <v>43</v>
       </c>
-      <c r="K37" s="16">
-        <f>SUM(K2:K36)</f>
-        <v>16.599</v>
+      <c r="K38" s="16">
+        <f>SUM(K2:K37)</f>
+        <v>16.728999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2111,6 +2158,6 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BoM crossing, cost down to 15$ (included PCBA fee)
</commit_message>
<xml_diff>
--- a/HW/Product/BoM/PIC16DevKit.xlsx
+++ b/HW/Product/BoM/PIC16DevKit.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\SAMPIDevKit\PIC16DevKit\PIC16F1887x\HW\Product\BoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16619367-4E6C-429E-9264-0DC93FC33B1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE374E4-9B8A-4041-A1E4-6BBEEB994125}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AC2C9739-183B-4393-85EE-4EA8A3EEC5E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{AC2C9739-183B-4393-85EE-4EA8A3EEC5E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Digikey" sheetId="1" r:id="rId1"/>
+    <sheet name="VN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="153">
   <si>
     <t>References</t>
   </si>
@@ -277,14 +278,222 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>CC0805ZKY5V6BB226</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R7BB104</t>
+  </si>
+  <si>
+    <t>TMCMB0J227MTRF</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R7BB105</t>
+  </si>
+  <si>
+    <t>AC0603JR-071KL</t>
+  </si>
+  <si>
+    <t>RT0603FRE0710KL</t>
+  </si>
+  <si>
+    <t>AC0603JR-074K7L</t>
+  </si>
+  <si>
+    <t>RC0603FR-0740K2L</t>
+  </si>
+  <si>
+    <t>RC0603FR-0775KL</t>
+  </si>
+  <si>
+    <t>AC0603JR-072K2L</t>
+  </si>
+  <si>
+    <t>AP2210N-3.3TRG1</t>
+  </si>
+  <si>
+    <t>MCP9700T-H/LT</t>
+  </si>
+  <si>
+    <t>SST25VF040B-50-4C-SAF</t>
+  </si>
+  <si>
+    <t>RV-3028-C7 32.768KHZ 1PPM-TA-QC</t>
+  </si>
+  <si>
+    <t>MP1470GJ-Z</t>
+  </si>
+  <si>
+    <t>PIC32MM0064GPM028-I/M6</t>
+  </si>
+  <si>
+    <t>74AVC2T45DC,125</t>
+  </si>
+  <si>
+    <t>PIC16F18876-I/PT</t>
+  </si>
+  <si>
+    <t>MIC5504-3.3YM5-TR</t>
+  </si>
+  <si>
+    <t>SSM3J378R,LF</t>
+  </si>
+  <si>
+    <t>150060BS75000</t>
+  </si>
+  <si>
+    <t>150060SS75000</t>
+  </si>
+  <si>
+    <t>150060VS75000</t>
+  </si>
+  <si>
+    <t>150060YS75000</t>
+  </si>
+  <si>
+    <t>1N4148WSTR</t>
+  </si>
+  <si>
+    <t>SK26_R1_00001</t>
+  </si>
+  <si>
+    <t>PTS810 SJG 250 SMTR LFS</t>
+  </si>
+  <si>
+    <t>0ZCG0050AF2C</t>
+  </si>
+  <si>
+    <t>10118192-0002LF</t>
+  </si>
+  <si>
+    <t>RS1-10-G</t>
+  </si>
+  <si>
+    <t>RS1-07-G</t>
+  </si>
+  <si>
+    <t>RS1-08-G</t>
+  </si>
+  <si>
+    <t>HRS-2B-10-GA</t>
+  </si>
+  <si>
+    <t>SDE0604A-6R8M</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/tu-gom-0805-22uf-16v</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/tu-gom-0603-100nf-0-1uf-25v</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/tu-gom-0603-1uf-50v</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/tu-tantalum-220uf-6-3v-1210-f930j227mba</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-1-kohm-0603-1</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-10-kohm-0603-1</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-4-7-kohm-0603-5</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-40-2-kohm-0603-1</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-75-kohm-0603-1</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/dien-tro-2-2-kohm-0603-5</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/mcp1700t-3302e-ic-on-ap-3-3v-250ma</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/mcp9700at-e-tt-cam-bien-nhiet-do</t>
+  </si>
+  <si>
+    <t>https://store.rpc.vn/sst25vf040b-80-4i-s2ae?search=SST25VF040</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/micro-crystal-ag/RV-3028-C7-32-768KHZ-1PPM-TA-QC/10431070</t>
+  </si>
+  <si>
+    <t>https://banlinhkien.com/mp1470-sot23-ic-buck-2a-16v-adjgadje-p6648672.html</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/PIC32MM0064GPM028-I-M6/8037777</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/74AVC2T45DC-125/1692558</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/PIC16F18876-I-PT/6192935</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/rt9193-33gb-ic-on-ap-3-3v-300ma</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/si2301ds</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/led-xanh-duong-0603-dan-smd-trong-suot</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/led-do-0603-dan-smd-trong-suot</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/led-xanh-la-0603-dan-smd-trong-suot</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/led-vang-0603-dan-smd-trong-suot</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/1n4148ws-diode-chinh-luu-0-15a-75v</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/ss24-sma</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/nut-nhan-4-2x3-3mm-cao-2-5mm-4-chan-smd-v2</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/mf-msmf075-24-2-cau-chi-tu-phuc-hoi-1812-24v-0-75a</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/cong-usb-micro-b-2-0-dau-cai-5-chan-smd-v3</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/hang-rao-cai-don-2-54mm-40-chan-1-hang-cao-11-8mm-xuyen-lo</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/hang-rao-cai-doi-1-27mm-80-chan-2-hang-cao-4-3mm-xuyen-lo</t>
+  </si>
+  <si>
+    <t>https://www.thegioiic.com/products/cuon-cam-dan-smd-cd53-5852-6r8-6-8uh-2-2a</t>
+  </si>
+  <si>
+    <t>PCBA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="[$VND]\ #,##0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -333,7 +542,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -382,12 +591,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -404,7 +650,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -422,12 +668,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -440,11 +680,51 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -766,9 +1046,9 @@
   </sheetPr>
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N37" sqref="A1:N37"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,14 +1092,14 @@
       <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="12" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="13"/>
+      <c r="L1" s="19"/>
       <c r="M1" s="4" t="s">
         <v>2</v>
       </c>
@@ -2296,32 +2576,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+    <row r="37" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="13">
         <f>SUM(B2:B36)</f>
         <v>73</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17">
+      <c r="C37" s="12"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15">
         <f>SUM(J2:J36)</f>
         <v>247</v>
       </c>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17">
+      <c r="K37" s="15"/>
+      <c r="L37" s="15">
         <f>SUM(L2:L36)</f>
         <v>47</v>
       </c>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18">
+      <c r="M37" s="16"/>
+      <c r="N37" s="16">
         <f>SUM(N2:N36)</f>
         <v>21.801999999999996</v>
       </c>
@@ -2335,4 +2615,1076 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C20ADDC-FEA2-4693-9F5F-7160D9A03DCF}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="87" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="101.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20">
+        <v>1120</v>
+      </c>
+      <c r="G2" s="20">
+        <f>B2*F2</f>
+        <v>6720</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="20">
+        <v>218</v>
+      </c>
+      <c r="G3" s="20">
+        <f t="shared" ref="G3:G37" si="0">B3*F3</f>
+        <v>3488</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="20">
+        <v>3400</v>
+      </c>
+      <c r="G4" s="20">
+        <f t="shared" si="0"/>
+        <v>6800</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="20">
+        <v>280</v>
+      </c>
+      <c r="G5" s="20">
+        <f t="shared" si="0"/>
+        <v>840</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="20">
+        <v>46</v>
+      </c>
+      <c r="G6" s="20">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="20">
+        <v>46</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="20">
+        <v>32</v>
+      </c>
+      <c r="G8" s="20">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="20">
+        <v>46</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="20">
+        <v>46</v>
+      </c>
+      <c r="G10" s="20">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="20">
+        <v>32</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="20">
+        <v>6900</v>
+      </c>
+      <c r="G12" s="20">
+        <f t="shared" si="0"/>
+        <v>6900</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="20">
+        <v>6000</v>
+      </c>
+      <c r="G13" s="20">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="20">
+        <v>23887</v>
+      </c>
+      <c r="G14" s="20">
+        <f t="shared" si="0"/>
+        <v>23887</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="20">
+        <v>72485</v>
+      </c>
+      <c r="G15" s="20">
+        <f t="shared" si="0"/>
+        <v>72485</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="20">
+        <v>4000</v>
+      </c>
+      <c r="G16" s="20">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="20">
+        <v>52186</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" si="0"/>
+        <v>52186</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="20">
+        <v>12791</v>
+      </c>
+      <c r="G18" s="20">
+        <f t="shared" si="0"/>
+        <v>12791</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="20">
+        <v>43233</v>
+      </c>
+      <c r="G19" s="20">
+        <f t="shared" si="0"/>
+        <v>43233</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="20">
+        <v>3600</v>
+      </c>
+      <c r="G20" s="20">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="20">
+        <v>500</v>
+      </c>
+      <c r="G21" s="20">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="20">
+        <v>290</v>
+      </c>
+      <c r="G22" s="20">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="20">
+        <v>180</v>
+      </c>
+      <c r="G23" s="20">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="20">
+        <v>290</v>
+      </c>
+      <c r="G24" s="20">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="20">
+        <v>200</v>
+      </c>
+      <c r="G25" s="20">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
+      <c r="B26" s="11">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="20">
+        <v>510</v>
+      </c>
+      <c r="G26" s="20">
+        <f t="shared" si="0"/>
+        <v>510</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>26</v>
+      </c>
+      <c r="B27" s="11">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="20">
+        <v>960</v>
+      </c>
+      <c r="G27" s="20">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="20">
+        <v>800</v>
+      </c>
+      <c r="G28" s="20">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>28</v>
+      </c>
+      <c r="B29" s="11">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="20">
+        <v>3500</v>
+      </c>
+      <c r="G29" s="20">
+        <f t="shared" si="0"/>
+        <v>3500</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="20">
+        <v>800</v>
+      </c>
+      <c r="G30" s="20">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>30</v>
+      </c>
+      <c r="B31" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="20">
+        <v>2000</v>
+      </c>
+      <c r="G31" s="20">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H31" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="24">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="20">
+        <v>2000</v>
+      </c>
+      <c r="G32" s="20">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="20">
+        <v>2000</v>
+      </c>
+      <c r="G33" s="20">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="H33" s="28"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>33</v>
+      </c>
+      <c r="B34" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="20">
+        <v>10800</v>
+      </c>
+      <c r="G34" s="20">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>34</v>
+      </c>
+      <c r="B35" s="11">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="20">
+        <v>2400</v>
+      </c>
+      <c r="G35" s="20">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="11">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="20">
+        <v>24000</v>
+      </c>
+      <c r="G36" s="20">
+        <f t="shared" si="0"/>
+        <v>24000</v>
+      </c>
+      <c r="H36" s="29"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>36</v>
+      </c>
+      <c r="B37" s="11">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="20">
+        <f>0.25*SUM(G2:G36)</f>
+        <v>71004</v>
+      </c>
+      <c r="G37" s="20">
+        <f t="shared" si="0"/>
+        <v>71004</v>
+      </c>
+      <c r="H37" s="31"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="13">
+        <f>SUM(B2:B37)</f>
+        <v>70.125</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21">
+        <f>SUM(G2:G37)</f>
+        <v>355020</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H31:H33"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{167FD2B5-6396-4B9D-BECA-ACDF4E42C0D5}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{2F0E2676-F4C4-4EC1-84EF-6624EFF86AD8}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{1F32BE7A-807A-4BFC-94D8-78A0C5713279}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{FB38A6C0-600C-4AC4-9DAA-C51E2D977483}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{44CF8FC3-43AE-4AB5-8585-033D1EE88EBE}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{726A86DE-B12E-4974-8E86-F735A6BDBAAE}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{73DD48EA-CA51-4F1D-87BE-24343420FD3A}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{533942F0-1A6B-473B-BCD9-3C46E8E3B5B5}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{8392403F-38B5-4513-903B-C6C1875AD52D}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{36CFA50C-1BE6-4C6A-B78E-36DF8E8E1AA4}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{F7BF691F-B673-44D3-8C79-7812DDF3F039}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{9DEA2EF8-F4ED-4B55-ADAF-AD0ABD50A2FD}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{EDC945B5-539E-455C-85D8-B7AFCBB10518}"/>
+    <hyperlink ref="H15" r:id="rId14" xr:uid="{0048F2F4-C599-4807-8CFE-850000D56084}"/>
+    <hyperlink ref="H16" r:id="rId15" xr:uid="{2FCCDB05-DD84-4FF1-BA80-BEB47EF9E0B7}"/>
+    <hyperlink ref="H17" r:id="rId16" xr:uid="{37C5A5F9-B286-4AAD-970E-3CB8932D45E2}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{469AF33D-2A8A-4387-91CF-5AA4187D2CB0}"/>
+    <hyperlink ref="H19" r:id="rId18" xr:uid="{59C8B3D7-A677-4B83-99FF-C65F61D24E0A}"/>
+    <hyperlink ref="H20" r:id="rId19" xr:uid="{C96D3580-11AA-403E-BECC-18025597B39F}"/>
+    <hyperlink ref="H21" r:id="rId20" xr:uid="{9F08AB65-0690-4BFA-B127-6748EEF5ED1D}"/>
+    <hyperlink ref="H22" r:id="rId21" xr:uid="{7F9D88F7-ECE3-47E5-B3E5-AC44967BBAC0}"/>
+    <hyperlink ref="H23" r:id="rId22" xr:uid="{03D2648C-876E-449E-BB5E-7A7B479D9CC4}"/>
+    <hyperlink ref="H24" r:id="rId23" xr:uid="{7E7FC8B9-5CD6-4332-A714-B39499D59A41}"/>
+    <hyperlink ref="H25" r:id="rId24" xr:uid="{D78930E7-3A9C-4FD3-B20F-3FEE966EE944}"/>
+    <hyperlink ref="H26" r:id="rId25" xr:uid="{A48F5738-7DC0-4669-8B5A-805432A7EADD}"/>
+    <hyperlink ref="H27" r:id="rId26" xr:uid="{5C21A789-3AD6-4B32-814C-274ABA558ECB}"/>
+    <hyperlink ref="H28" r:id="rId27" xr:uid="{75A39B23-BBAF-4997-849A-5693B45568C6}"/>
+    <hyperlink ref="H29" r:id="rId28" xr:uid="{D3E37834-3685-4774-BB92-5BC9B6B2E586}"/>
+    <hyperlink ref="H30" r:id="rId29" xr:uid="{C47DE938-D145-4429-9846-9D5DAE670935}"/>
+    <hyperlink ref="H31" r:id="rId30" xr:uid="{32B17B76-FAE1-4BB3-B08E-003D13474661}"/>
+    <hyperlink ref="H34" r:id="rId31" xr:uid="{744E2E6D-F5C2-4326-A693-1A429C378DB0}"/>
+    <hyperlink ref="H35" r:id="rId32" xr:uid="{5B30E04F-4550-4E43-87F9-22A384C301A1}"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="landscape" r:id="rId33"/>
+</worksheet>
 </file>
</xml_diff>